<commit_message>
Updated delegate and template
</commit_message>
<xml_diff>
--- a/clients/DiveInsurance/data/template/Phly_IL.xlsx
+++ b/clients/DiveInsurance/data/template/Phly_IL.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Cert #</t>
   </si>
@@ -70,6 +70,12 @@
     <t>Cancel_Date</t>
   </si>
   <si>
+    <t>Reinstated</t>
+  </si>
+  <si>
+    <t>Reinstate_date</t>
+  </si>
+  <si>
     <t>Upgrade</t>
   </si>
   <si>
@@ -158,6 +164,12 @@
   </si>
   <si>
     <t>{{cancel_date}}</t>
+  </si>
+  <si>
+    <t>{{reinstated}}</t>
+  </si>
+  <si>
+    <t>{{reinstated_date}}</t>
   </si>
   <si>
     <t>{{upgrade}}</t>
@@ -509,7 +521,7 @@
   <cols>
     <col customWidth="1" min="13" max="13" width="19.71"/>
     <col customWidth="1" min="14" max="15" width="18.86"/>
-    <col customWidth="1" min="28" max="28" width="15.86"/>
+    <col customWidth="1" min="30" max="30" width="15.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -588,112 +600,124 @@
       <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" s="4" t="s">
         <v>29</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AB2" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AC2" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AD2" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3">

</xml_diff>